<commit_message>
Markdown formatting of NEWS
</commit_message>
<xml_diff>
--- a/datatables/convert_clearance_types.xlsx
+++ b/datatables/convert_clearance_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wambaugh_john_epa_gov/Documents/Profile/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C5D308-D06E-466E-B324-60C593E3C984}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{543B3870-AD34-4355-876E-483B146453F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C71D3DA-CD9D-4A3C-922E-78D67B5DB213}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67E38929-52AA-449F-9892-ABB9AC15BB39}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67E38929-52AA-449F-9892-ABB9AC15BB39}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Parameter</t>
   </si>
@@ -197,16 +200,43 @@
   </si>
   <si>
     <t>Units5</t>
+  </si>
+  <si>
+    <t>amount per gram liver</t>
+  </si>
+  <si>
+    <t>gram liver per mL liver</t>
+  </si>
+  <si>
+    <t>L liver per kg body weight</t>
+  </si>
+  <si>
+    <t>amount per gram liver2</t>
+  </si>
+  <si>
+    <t>gram liver per mL liver3</t>
+  </si>
+  <si>
+    <t>L liver per kg body weight4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -249,16 +279,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="29">
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -266,40 +355,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -340,41 +396,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{249CA7ED-28D0-48ED-B825-FAA20C91112B}" name="Table2" displayName="Table2" ref="A1:L5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L5" xr:uid="{3778A077-6B41-4C7D-AE0B-9C0291B35A38}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9785AA5A-D815-4009-A982-90D166BC7FC0}" name="Measurement" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{D8329403-D9B1-41CA-B8E8-57D037AEA581}" name="Method" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{5F2C2FE3-600F-422C-BA19-F5009B449DCF}" name="Units" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{91EA77BE-8AF9-4D81-BD3C-153087ADBAFA}" name="Value" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{B1A31905-0F5E-4BD5-9B4F-271A1B0A88CB}" name="Human Cl_int_hep" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{5BE9CB23-5551-4488-8010-B46946432C5C}" name="Units2" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{DFCD18C5-CD14-401D-A0C9-4DA087E54841}" name="Human Hepatic Clearance (Cl_h)" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{249CA7ED-28D0-48ED-B825-FAA20C91112B}" name="Table2" displayName="Table2" ref="A1:R5" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:R5" xr:uid="{3778A077-6B41-4C7D-AE0B-9C0291B35A38}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{9785AA5A-D815-4009-A982-90D166BC7FC0}" name="Measurement" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{D8329403-D9B1-41CA-B8E8-57D037AEA581}" name="Method" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{5F2C2FE3-600F-422C-BA19-F5009B449DCF}" name="Units" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{91EA77BE-8AF9-4D81-BD3C-153087ADBAFA}" name="Value" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{B1A31905-0F5E-4BD5-9B4F-271A1B0A88CB}" name="Human Cl_int_hep" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{5BE9CB23-5551-4488-8010-B46946432C5C}" name="Units2" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{2307CEC8-52A3-43BD-9E01-159FFA2CC02F}" name="amount per gram liver" dataDxfId="6">
+      <calculatedColumnFormula>Constants!D4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{397759AB-7CBD-45D4-9D23-392866F0CBC7}" name="gram liver per mL liver" dataDxfId="5">
+      <calculatedColumnFormula>Constants!$D$6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{7E8747D5-E547-414C-AB47-E8533CE17190}" name="L liver per kg body weight" dataDxfId="4">
+      <calculatedColumnFormula>Constants!$D$5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DFCD18C5-CD14-401D-A0C9-4DA087E54841}" name="Human Hepatic Clearance (Cl_h)" dataDxfId="20">
       <calculatedColumnFormula>Constants!$D$4*Constants!$D$8*Constants!$D$6*Factors!D2/1000*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{248D6BAD-7A6F-4718-AF84-B1837681292D}" name="Units3" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{848F52A6-5AE7-40DA-BAE0-CAFE8DF2627F}" name="Rat Cl_int_hep" dataDxfId="0">
-      <calculatedColumnFormula>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/K$2</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{248D6BAD-7A6F-4718-AF84-B1837681292D}" name="Units3" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{848F52A6-5AE7-40DA-BAE0-CAFE8DF2627F}" name="Rat Cl_int_hep" dataDxfId="18">
+      <calculatedColumnFormula>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/Q$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{444FE854-895F-41D3-961B-5BA91D000F68}" name="Units4" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{E0A104EB-B44D-4837-900C-56627F0C1FB3}" name="Rag Hepatic Clearance (Cl_h)4" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{C618CC55-DBCA-48A1-9A75-B8842276BFA6}" name="Units5" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{444FE854-895F-41D3-961B-5BA91D000F68}" name="Units4" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{3ABEDC50-01D9-48FF-9E72-87AB3C603E82}" name="amount per gram liver2" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{99EAC3FF-A287-4093-9DD9-445E47DD8380}" name="gram liver per mL liver3" dataDxfId="2">
+      <calculatedColumnFormula>Constants!$F$6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{E1709A60-F054-476F-9CD3-7F9837A098F5}" name="L liver per kg body weight4" dataDxfId="1">
+      <calculatedColumnFormula>Constants!$F$5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{E0A104EB-B44D-4837-900C-56627F0C1FB3}" name="Rag Hepatic Clearance (Cl_h)4" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{C618CC55-DBCA-48A1-9A75-B8842276BFA6}" name="Units5" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0DD49C9-D53E-4D2A-83CA-115035DA6072}" name="Table1" displayName="Table1" ref="A1:G8" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0DD49C9-D53E-4D2A-83CA-115035DA6072}" name="Table1" displayName="Table1" ref="A1:G8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:G8" xr:uid="{0312A655-0213-43D6-942E-BF5A4DA157B5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ED808134-76AA-470C-90D1-CB2DB393044B}" name="Parameter" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{2D7D49AF-D8F3-4792-8191-0AA37C908DCF}" name="Description" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{9D95A3AB-6BBF-4008-9273-F86D82411351}" name="Units" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{6471E546-9F59-45F7-B303-6F66E3FF3AAB}" name=" Mean Human Value (*Varied by HTTK-pop (Ring, et al., 2017))" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{372D8E51-6296-4D17-9CB0-0916F3960837}" name="Reference" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{12365BA6-E377-4FEE-9ABF-2B7DDE7D275C}" name="Mean Rat Value" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{D999C1BC-C4EC-4AE7-9B4D-91A784233CBC}" name="Reference2" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{ED808134-76AA-470C-90D1-CB2DB393044B}" name="Parameter" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2D7D49AF-D8F3-4792-8191-0AA37C908DCF}" name="Description" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{9D95A3AB-6BBF-4008-9273-F86D82411351}" name="Units" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{6471E546-9F59-45F7-B303-6F66E3FF3AAB}" name=" Mean Human Value (*Varied by HTTK-pop (Ring, et al., 2017))" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{372D8E51-6296-4D17-9CB0-0916F3960837}" name="Reference" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{12365BA6-E377-4FEE-9ABF-2B7DDE7D275C}" name="Mean Rat Value" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{D999C1BC-C4EC-4AE7-9B4D-91A784233CBC}" name="Reference2" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,23 +749,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42558E92-9B8E-4BC8-A35A-66ED626FB405}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="1" max="2" width="15.53515625" customWidth="1"/>
+    <col min="3" max="3" width="19.69140625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="6" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="24.69140625" customWidth="1"/>
+    <col min="11" max="11" width="13.69140625" customWidth="1"/>
+    <col min="16" max="16" width="11.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -713,25 +786,43 @@
         <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -745,35 +836,59 @@
         <v>1</v>
       </c>
       <c r="E2" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/G$2</f>
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/J$2</f>
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="3">
-        <f>Constants!$D$4*Constants!$D$5*Constants!$D$6*Factors!D2/10^6*60*1000</f>
+      <c r="G2" s="1">
+        <f>Constants!$D$4</f>
+        <v>110</v>
+      </c>
+      <c r="H2" s="1">
+        <f>Constants!$D$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="I2" s="1">
+        <f>Constants!$D$5</f>
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="J2" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/10^6*60*1000</f>
         <v>0.16978500000000002</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/K$2</f>
+      <c r="L2" s="3">
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/Q$2</f>
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="3">
-        <f>Constants!$F$4*Constants!$D$5*Constants!$F$6*Factors!D2/10^6*60*1000</f>
+      <c r="N2" s="1">
+        <f>Constants!$F$4</f>
+        <v>110</v>
+      </c>
+      <c r="O2" s="1">
+        <f>Constants!$F$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="P2" s="6">
+        <f>Constants!$F$5</f>
+        <v>3.4857142857142857E-2</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/10^6*60*1000</f>
         <v>0.16978500000000002</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -787,35 +902,59 @@
         <v>1</v>
       </c>
       <c r="E3" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/G$2</f>
-        <v>30.612244897959179</v>
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/J$2</f>
+        <v>6.8181818181818187E-3</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="3">
-        <f>Constants!$D$4*Constants!$D$8*Constants!$D$6*Factors!D3/1000</f>
-        <v>5.1974999999999998</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="1">
+        <f>Constants!$D$8</f>
+        <v>45</v>
+      </c>
+      <c r="H3" s="1">
+        <f>Constants!$D$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="I3" s="1">
+        <f>Constants!$D$5</f>
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/1000</f>
+        <v>1.1576250000000002E-3</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/K$2</f>
-        <v>30.612244897959179</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="3">
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/Q$2</f>
+        <v>6.8181818181818187E-3</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="3">
-        <f>Constants!$F$4*Constants!$F$8*Constants!$F$6*Factors!D3/1000</f>
-        <v>5.1974999999999998</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1">
+        <f>Constants!$F$8</f>
+        <v>45</v>
+      </c>
+      <c r="O3" s="1">
+        <f>Constants!$F$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="P3" s="6">
+        <f>Constants!$F$5</f>
+        <v>3.4857142857142857E-2</v>
+      </c>
+      <c r="Q3" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/1000</f>
+        <v>1.1576250000000002E-3</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -829,35 +968,59 @@
         <v>1</v>
       </c>
       <c r="E4" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/G$2</f>
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/J$2</f>
         <v>16.666666666666664</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="3">
-        <f>Constants!$D$4*Constants!$D$5*Constants!$D$6*Factors!D4/10^3*1000</f>
+      <c r="G4" s="1">
+        <f>Constants!$D$4</f>
+        <v>110</v>
+      </c>
+      <c r="H4" s="1">
+        <f>Constants!$D$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="I4" s="1">
+        <f>Constants!$D$5</f>
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/10^3*1000</f>
         <v>2.8297500000000002</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/K$2</f>
+      <c r="L4" s="3">
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/Q$2</f>
         <v>16.666666666666664</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="3">
-        <f>Constants!$F$4*Constants!$F$5*Constants!$F$6*Factors!D4/10^3*1000</f>
-        <v>4.0260000000000007</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1">
+        <f>Constants!$F$4</f>
+        <v>110</v>
+      </c>
+      <c r="O4" s="1">
+        <f>Constants!$F$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="P4" s="6">
+        <f>Constants!$F$5</f>
+        <v>3.4857142857142857E-2</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/10^3*1000</f>
+        <v>2.8297500000000002</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -871,35 +1034,60 @@
         <v>1</v>
       </c>
       <c r="E5" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/G$2</f>
-        <v>1.8367346938775508</v>
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/J$2</f>
+        <v>4.0909090909090913E-4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="3">
-        <f>Constants!$D$4*Constants!$D$8*Constants!$D$6*Factors!D5/1000/1000*60</f>
-        <v>0.31185000000000002</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="G5" s="1">
+        <f>Constants!$D$8</f>
+        <v>45</v>
+      </c>
+      <c r="H5" s="1">
+        <f>Constants!$D$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="I5" s="1">
+        <f>Constants!$D$5</f>
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/1000/1000*60</f>
+        <v>6.9457500000000017E-5</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="3">
-        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/K$2</f>
-        <v>1.8367346938775508</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="3">
+        <f>Table2[[#This Row],[Human Hepatic Clearance (Cl_h)]]/Q$2</f>
+        <v>4.0909090909090913E-4</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="3">
-        <f>Constants!$F$4*Constants!$F$8*Constants!$F$6*Factors!D5/1000/1000*60</f>
-        <v>0.31185000000000002</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1">
+        <f>Constants!$F$8</f>
+        <v>45</v>
+      </c>
+      <c r="O5" s="1">
+        <f>Constants!$F$6</f>
+        <v>1.05</v>
+      </c>
+      <c r="P5" s="6">
+        <f>Constants!$F$5</f>
+        <v>3.4857142857142857E-2</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>Table2[[#This Row],[Value]]*Table2[[#This Row],[amount per gram liver]]*Table2[[#This Row],[gram liver per mL liver]]*Table2[[#This Row],[L liver per kg body weight]]/1000/1000*60</f>
+        <v>6.9457500000000017E-5</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -911,20 +1099,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158BCB52-56FD-4263-BE98-76E3EB844A28}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" customWidth="1"/>
+    <col min="2" max="2" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="50.53515625" customWidth="1"/>
+    <col min="5" max="5" width="12.3046875" customWidth="1"/>
+    <col min="6" max="6" width="11.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +1135,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -971,7 +1159,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -995,7 +1183,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1018,7 +1206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1041,7 +1229,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1064,7 +1252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1087,7 +1275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>